<commit_message>
was able to output sections 1-4
</commit_message>
<xml_diff>
--- a/outputExcel.xlsx
+++ b/outputExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1551b3744a113d45/Documents/UiPath/Robotic_Process_Automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="216" documentId="8_{0129B809-5A3B-48E5-AC84-8C2BCB68F3C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BC9271E5-F53B-4DF3-ADB9-8FB4C9A0907C}"/>
+  <xr:revisionPtr revIDLastSave="488" documentId="8_{0129B809-5A3B-48E5-AC84-8C2BCB68F3C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F7B18009-5E39-4715-9D9F-271B75025003}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{D33220B9-F8AC-4806-9C5E-F53489A6E462}"/>
   </bookViews>
@@ -35,111 +35,144 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
+  <si>
+    <t xml:space="preserve">Jan-20  Change Monitoring Monthly Review      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">On a monthly basis, IT R&amp;C manager will conduct a review of the weekly reviews executed by IT R&amp;C analysist. The manager review is executed to make sure all servers and all days within the month are accounted for. Additionally, the manager haphazardly selected 5 days within the month and re-executes the review to ensure the procedures were accurately performed. If any discrepancies are identified, the manager performs further investigation.        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Template found here: \\MainFolder\Daily_Change_Monitoring\Monthly Manager Review        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Review monthly monitoring tracker and ensure all days were monitored by analyst.        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">a. Access the monthly monitor tracker at:        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">i. \\MainFolder\Daily_Change_Monitoring        </t>
+  </si>
+  <si>
+    <t>b. The Daily Change Monitoring tracker will contain a 'days tracked tab'. All days tracked will contain an "X" for that day or the ServiceNow ticket associated with the change for that day</t>
+  </si>
+  <si>
+    <t>Step 1 Review Sign off ___________</t>
+  </si>
+  <si>
+    <t>2. From the Findings Tracker tab, haphazardly select a numer of days (from population of monthly days found on the days track tab) and ensure an email was</t>
+  </si>
+  <si>
+    <t>received for each server on the days selected.</t>
+  </si>
+  <si>
+    <t>a. All emails are archived by date at: \\MainFolder\Daily_Change_Monitoring\</t>
+  </si>
+  <si>
+    <t>Selection 1 (date)</t>
+  </si>
+  <si>
+    <t>Emails Received</t>
+  </si>
+  <si>
+    <t>Selection 2 (date)</t>
+  </si>
+  <si>
+    <t>Step 2 Review Sign off ___________</t>
+  </si>
+  <si>
+    <t>"3. For the days selected in step two, identify all emails which denote a change detected. Open each email and ensure the details within (e.g. each change is captured within the monthly tracker (findings tab)."</t>
+  </si>
+  <si>
+    <t>Selection 1 (Date)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Total Changes</t>
+  </si>
+  <si>
+    <t>magic_qq_appl</t>
+  </si>
+  <si>
+    <t>testps01</t>
+  </si>
+  <si>
+    <t>testps0324</t>
+  </si>
+  <si>
+    <t>testps9023</t>
+  </si>
+  <si>
+    <t>Selection 2 (Date)</t>
+  </si>
+  <si>
+    <t>magic435</t>
+  </si>
+  <si>
+    <t>magic_qq_23455</t>
+  </si>
+  <si>
+    <t>test_2348q</t>
+  </si>
+  <si>
+    <t>test234234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. From the Findings Tracker tab, haphazardly select five changes that occurred (and have a </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ServiceNow ticket identified). For each change, ensure the ServiceNow ticker referenced </t>
+  </si>
+  <si>
+    <t>appropriately maps to the identified change.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a. The ServiceNow ticket names can be found in the 'Conclusion Evidence Name' column located in </t>
+  </si>
+  <si>
+    <t>the Findings Tracker tab.</t>
+  </si>
+  <si>
+    <t>b. Access the Remediation and Justification Evidence for any changes at: \\MainFolder</t>
+  </si>
+  <si>
+    <t>\\Remediation_or_Justification Evidence</t>
+  </si>
+  <si>
+    <t>Step 4 Review Sign off ___________</t>
+  </si>
+  <si>
+    <t>C:\Users\karth\OneDrive\Documents\UiPath\Robotic_Process_Automation\FOLDER\Mainfolder\Daily_Change_Monitoring\1Jan2020\01-09-2020\*</t>
+  </si>
+  <si>
+    <t>C:\Users\karth\OneDrive\Documents\UiPath\Robotic_Process_Automation\FOLDER\Mainfolder\Daily_Change_Monitoring\1Jan2020\01-22-2020\*</t>
+  </si>
+  <si>
+    <t>CHANGES - SOX Audit Report for magic_qq_appl.txt_07.01.73</t>
+  </si>
+  <si>
+    <t>CHANGES - SOX Audit Report for magic435.txt_07.01.73</t>
+  </si>
+  <si>
+    <t>CHANGES - SOX Audit Report for testps01.txt_07.01.73</t>
+  </si>
+  <si>
+    <t>CHANGES - SOX Audit Report for magic_qq_23455.txt_07.01.73</t>
+  </si>
   <si>
     <t>CHANGES - SOX Audit Report for testps0324.txt_07.01.73</t>
   </si>
   <si>
+    <t>CHANGES - SOX Audit Report for test234234.txt_07.01.73</t>
+  </si>
+  <si>
     <t>CHANGES - SOX Audit Report for testps9023.txt_07.01.73</t>
   </si>
   <si>
     <t>CHANGES - SOX Audit Report for test_2348q.txt_07.01.73</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jan-20  Change Monitoring Monthly Review      </t>
-  </si>
-  <si>
-    <t xml:space="preserve">On a monthly basis, IT R&amp;C manager will conduct a review of the weekly reviews executed by IT R&amp;C analysist. The manager review is executed to make sure all servers and all days within the month are accounted for. Additionally, the manager haphazardly selected 5 days within the month and re-executes the review to ensure the procedures were accurately performed. If any discrepancies are identified, the manager performs further investigation.        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Template found here: \\MainFolder\Daily_Change_Monitoring\Monthly Manager Review        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Review monthly monitoring tracker and ensure all days were monitored by analyst.        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">a. Access the monthly monitor tracker at:        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">i. \\MainFolder\Daily_Change_Monitoring        </t>
-  </si>
-  <si>
-    <t>b. The Daily Change Monitoring tracker will contain a 'days tracked tab'. All days tracked will contain an "X" for that day or the ServiceNow ticket associated with the change for that day</t>
-  </si>
-  <si>
-    <t>Step 1 Review Sign off ___________</t>
-  </si>
-  <si>
-    <t>C:\Users\karth\OneDrive\Documents\UiPath\Robotic_Process_Automation\FOLDER\Mainfolder\Daily_Change_Monitoring\1Jan2020\01-09-2020\*</t>
-  </si>
-  <si>
-    <t>C:\Users\karth\OneDrive\Documents\UiPath\Robotic_Process_Automation\FOLDER\Mainfolder\Daily_Change_Monitoring\1Jan2020\01-13-2020\*</t>
-  </si>
-  <si>
-    <t>CHANGES - SOX Audit Report for magic_qq_appl.txt_07.01.73</t>
-  </si>
-  <si>
-    <t>CHANGES - SOX Audit Report for testps01.txt_07.01.73</t>
-  </si>
-  <si>
-    <t>CHANGES - SOX Audit Report for magic_kl02.txt_07.01.73</t>
-  </si>
-  <si>
-    <t>CHANGES - SOX Audit Report for magic_kq_023.txt_07.01.73</t>
-  </si>
-  <si>
-    <t>2. From the Findings Tracker tab, haphazardly select a numer of days (from population of monthly days found on the days track tab) and ensure an email was</t>
-  </si>
-  <si>
-    <t>received for each server on the days selected.</t>
-  </si>
-  <si>
-    <t>a. All emails are archived by date at: \\MainFolder\Daily_Change_Monitoring\</t>
-  </si>
-  <si>
-    <t>Selection 1 (date)</t>
-  </si>
-  <si>
-    <t>Emails Received</t>
-  </si>
-  <si>
-    <t>Selection 2 (date)</t>
-  </si>
-  <si>
-    <t>Step 2 Review Sign off ___________</t>
-  </si>
-  <si>
-    <t>"3. For the days selected in step two, identify all emails which denote a change detected. Open each email and ensure the details within (e.g. each change is captured within the monthly tracker (findings tab)."</t>
-  </si>
-  <si>
-    <t>Selection 1 (Date)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Total Changes</t>
-  </si>
-  <si>
-    <t>magic_qq_appl</t>
-  </si>
-  <si>
-    <t>testps01</t>
-  </si>
-  <si>
-    <t>testps0324</t>
-  </si>
-  <si>
-    <t>testps9023</t>
-  </si>
-  <si>
-    <t>Selection 2 (Date)</t>
-  </si>
-  <si>
-    <t>magic_kq_023</t>
-  </si>
-  <si>
-    <t>magic_kl02</t>
   </si>
 </sst>
 </file>
@@ -175,9 +208,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,174 +527,220 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F11F7830-7076-47CD-ADA6-DB00BD6F2D35}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="S44" sqref="S44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="10.109375" customWidth="1"/>
-    <col min="5" max="5" width="10.77734375" customWidth="1"/>
+    <col min="1" max="3" width="9.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="2">
+        <v>43839</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="2">
+        <v>43852</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="D28" s="2">
+        <v>43839</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="G28" s="1">
+        <v>4</v>
+      </c>
+      <c r="H28" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C16" t="s">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H29" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="1">
-        <v>43839</v>
-      </c>
-      <c r="F16" t="s">
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H30" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H16">
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H31" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B32" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="2">
+        <v>43852</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G32" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C17" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" s="1">
-        <v>43843</v>
-      </c>
-      <c r="F17" t="s">
-        <v>21</v>
-      </c>
-      <c r="H17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="H32" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H33" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C28" t="s">
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H34" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D28" s="1">
-        <v>43839</v>
-      </c>
-      <c r="E28" t="s">
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H35" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G28">
-        <v>4</v>
-      </c>
-      <c r="H28" t="s">
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H29" t="s">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H30" t="s">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H31" t="s">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B32" t="s">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C32" t="s">
-        <v>26</v>
-      </c>
-      <c r="D32" s="1">
-        <v>43843</v>
-      </c>
-      <c r="E32" t="s">
-        <v>27</v>
-      </c>
-      <c r="G32">
-        <v>3</v>
-      </c>
-      <c r="H32" t="s">
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H33" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="34" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H34" t="s">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -674,49 +754,49 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B1" sqref="B1 B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" t="s">
-        <v>12</v>
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
+      <c r="A2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
+      <c r="A3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
+      <c r="A4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
+      <c r="A5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
almost integrated section 5's workflow
</commit_message>
<xml_diff>
--- a/outputExcel.xlsx
+++ b/outputExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1551b3744a113d45/Documents/UiPath/Robotic_Process_Automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="488" documentId="8_{0129B809-5A3B-48E5-AC84-8C2BCB68F3C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F7B18009-5E39-4715-9D9F-271B75025003}"/>
+  <xr:revisionPtr revIDLastSave="546" documentId="8_{0129B809-5A3B-48E5-AC84-8C2BCB68F3C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DB4001C0-DAB1-4257-A578-D70593D76DDD}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{D33220B9-F8AC-4806-9C5E-F53489A6E462}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
     <t xml:space="preserve">Jan-20  Change Monitoring Monthly Review      </t>
   </si>
@@ -94,31 +94,28 @@
     <t>Total Changes</t>
   </si>
   <si>
-    <t>magic_qq_appl</t>
-  </si>
-  <si>
-    <t>testps01</t>
-  </si>
-  <si>
-    <t>testps0324</t>
-  </si>
-  <si>
-    <t>testps9023</t>
+    <t>magic435</t>
+  </si>
+  <si>
+    <t>magic_qq_23455</t>
+  </si>
+  <si>
+    <t>test_2348q</t>
+  </si>
+  <si>
+    <t>test234234</t>
   </si>
   <si>
     <t>Selection 2 (Date)</t>
   </si>
   <si>
-    <t>magic435</t>
-  </si>
-  <si>
-    <t>magic_qq_23455</t>
-  </si>
-  <si>
-    <t>test_2348q</t>
-  </si>
-  <si>
-    <t>test234234</t>
+    <t>magic_iq23</t>
+  </si>
+  <si>
+    <t>testqcl12</t>
+  </si>
+  <si>
+    <t>oiuer3298</t>
   </si>
   <si>
     <t xml:space="preserve">4. From the Findings Tracker tab, haphazardly select five changes that occurred (and have a </t>
@@ -145,31 +142,28 @@
     <t>Step 4 Review Sign off ___________</t>
   </si>
   <si>
-    <t>C:\Users\karth\OneDrive\Documents\UiPath\Robotic_Process_Automation\FOLDER\Mainfolder\Daily_Change_Monitoring\1Jan2020\01-09-2020\*</t>
-  </si>
-  <si>
     <t>C:\Users\karth\OneDrive\Documents\UiPath\Robotic_Process_Automation\FOLDER\Mainfolder\Daily_Change_Monitoring\1Jan2020\01-22-2020\*</t>
   </si>
   <si>
-    <t>CHANGES - SOX Audit Report for magic_qq_appl.txt_07.01.73</t>
+    <t>C:\Users\karth\OneDrive\Documents\UiPath\Robotic_Process_Automation\FOLDER\Mainfolder\Daily_Change_Monitoring\1Jan2020\01-24-2020\*</t>
   </si>
   <si>
     <t>CHANGES - SOX Audit Report for magic435.txt_07.01.73</t>
   </si>
   <si>
-    <t>CHANGES - SOX Audit Report for testps01.txt_07.01.73</t>
+    <t>CHANGES - SOX Audit Report for magic_iq23.txt_07.01.73</t>
   </si>
   <si>
     <t>CHANGES - SOX Audit Report for magic_qq_23455.txt_07.01.73</t>
   </si>
   <si>
-    <t>CHANGES - SOX Audit Report for testps0324.txt_07.01.73</t>
+    <t>CHANGES - SOX Audit Report for oiuer3298.txt_07.01.73</t>
   </si>
   <si>
     <t>CHANGES - SOX Audit Report for test234234.txt_07.01.73</t>
   </si>
   <si>
-    <t>CHANGES - SOX Audit Report for testps9023.txt_07.01.73</t>
+    <t>CHANGES - SOX Audit Report for testqcl12.txt_07.01.73</t>
   </si>
   <si>
     <t>CHANGES - SOX Audit Report for test_2348q.txt_07.01.73</t>
@@ -527,10 +521,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F11F7830-7076-47CD-ADA6-DB00BD6F2D35}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="S44" sqref="S44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31 G31 A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -600,7 +594,7 @@
         <v>11</v>
       </c>
       <c r="E16" s="2">
-        <v>43839</v>
+        <v>43852</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>12</v>
@@ -614,13 +608,13 @@
         <v>13</v>
       </c>
       <c r="E17" s="2">
-        <v>43852</v>
+        <v>43854</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H17" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -641,7 +635,7 @@
         <v>17</v>
       </c>
       <c r="D28" s="2">
-        <v>43839</v>
+        <v>43852</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>18</v>
@@ -676,13 +670,13 @@
         <v>17</v>
       </c>
       <c r="D32" s="2">
-        <v>43852</v>
+        <v>43854</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>18</v>
       </c>
       <c r="G32" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>24</v>
@@ -699,7 +693,7 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H35" s="1" t="s">
+      <c r="A35" s="1" t="s">
         <v>27</v>
       </c>
     </row>
@@ -713,8 +707,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
         <v>30</v>
       </c>
     </row>
@@ -733,14 +727,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -761,42 +750,42 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed Server Name business exception error
</commit_message>
<xml_diff>
--- a/outputExcel.xlsx
+++ b/outputExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\Documents\UiPath\Robotic_Process_Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F38300F-1DC3-4101-B9FA-9028F4126447}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34C5E679-DAB9-4574-9169-D3693D587603}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10650" yWindow="7155" windowWidth="25050" windowHeight="13560" xr2:uid="{059AD380-688B-4FD3-B79B-167F2342754E}"/>
+    <workbookView xWindow="10650" yWindow="7155" windowWidth="25050" windowHeight="13560" activeTab="1" xr2:uid="{059AD380-688B-4FD3-B79B-167F2342754E}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="61">
   <si>
     <t>1/13/2020</t>
   </si>
@@ -575,7 +575,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -667,9 +667,9 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A0831D3-7B1D-497F-8861-303C38401867}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
@@ -942,6 +942,101 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>39</v>
+      </c>
+      <c r="E50" s="2">
+        <v>43839</v>
+      </c>
+      <c r="F50" t="s">
+        <v>40</v>
+      </c>
+      <c r="H50">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>41</v>
+      </c>
+      <c r="E51" s="2">
+        <v>43843</v>
+      </c>
+      <c r="F51" t="s">
+        <v>40</v>
+      </c>
+      <c r="H51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>42</v>
+      </c>
+      <c r="E52" s="2">
+        <v>43844</v>
+      </c>
+      <c r="F52" t="s">
+        <v>40</v>
+      </c>
+      <c r="H52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>43</v>
+      </c>
+      <c r="E53" s="2">
+        <v>43852</v>
+      </c>
+      <c r="F53" t="s">
+        <v>40</v>
+      </c>
+      <c r="H53">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>44</v>
+      </c>
+      <c r="E54" s="2">
+        <v>43854</v>
+      </c>
+      <c r="F54" t="s">
+        <v>40</v>
+      </c>
+      <c r="H54">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>